<commit_message>
arquivos criados para controle do bd
</commit_message>
<xml_diff>
--- a/dados_produtos.xlsx
+++ b/dados_produtos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D105"/>
+  <dimension ref="A1:E105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +442,11 @@
           <t>Valor do Produto</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>ICMS</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">

</xml_diff>